<commit_message>
add a new function to exceloutput.py
</commit_message>
<xml_diff>
--- a/src/models/file_importing/output.xlsx
+++ b/src/models/file_importing/output.xlsx
@@ -86,7 +86,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -102,6 +102,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF800000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -111,7 +119,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -119,13 +127,102 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -503,13 +600,13 @@
       <c r="B3">
         <v>1</v>
       </c>
-      <c r="C3" s="1">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1">
-        <v>1</v>
-      </c>
-      <c r="E3">
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="4">
         <v>1</v>
       </c>
       <c r="F3">
@@ -538,13 +635,13 @@
       <c r="B4">
         <v>1</v>
       </c>
-      <c r="C4" s="1">
-        <v>1</v>
-      </c>
-      <c r="D4" s="1">
-        <v>1</v>
-      </c>
-      <c r="E4">
+      <c r="C4" s="5">
+        <v>1</v>
+      </c>
+      <c r="D4" s="6">
+        <v>1</v>
+      </c>
+      <c r="E4" s="7">
         <v>1</v>
       </c>
       <c r="F4">
@@ -573,13 +670,13 @@
       <c r="B5">
         <v>1</v>
       </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
+      <c r="C5" s="8">
+        <v>1</v>
+      </c>
+      <c r="D5" s="9">
+        <v>1</v>
+      </c>
+      <c r="E5" s="10">
         <v>1</v>
       </c>
       <c r="F5">

</xml_diff>